<commit_message>
Removing progressively Macleod table
</commit_message>
<xml_diff>
--- a/Potential.establishment.KG_Configuration.xlsx
+++ b/Potential.establishment.KG_Configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maioran\Documents\Projects\Potential_establishment_KG - Leptinotarsa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maioran\Documents\Projects\Potential-establishment-KG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DDF988-D2FF-4998-94A2-A4DFEF2719B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E345B74B-586E-4962-8758-B535C5BE3AB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
   <si>
     <t>Present, no details</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>UK</t>
+  </si>
+  <si>
+    <t>Recalculate EU27 Climate list</t>
   </si>
 </sst>
 </file>
@@ -978,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF26EFA2-9019-4F6D-83AA-2B168DCBB3B9}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -1383,10 +1386,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,6 +1421,14 @@
       </c>
       <c r="B3" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New version. MacLeod excel table removed: climates are extracted directly from Koppen-Geiger map.
This is Leptinotarsa decemlineata specific version
</commit_message>
<xml_diff>
--- a/Potential.establishment.KG_Configuration.xlsx
+++ b/Potential.establishment.KG_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maioran\Documents\Projects\Potential-establishment-KG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E345B74B-586E-4962-8758-B535C5BE3AB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8492B5-D63F-424F-B2FF-1CA8369CD2E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -19,14 +19,26 @@
     <sheet name="Host_status_to_be_removed" sheetId="3" r:id="rId4"/>
     <sheet name="Protected_zones" sheetId="7" r:id="rId5"/>
     <sheet name="Other settings" sheetId="4" r:id="rId6"/>
-    <sheet name="tech" sheetId="6" r:id="rId7"/>
+    <sheet name="Climates_to_remove" sheetId="8" r:id="rId7"/>
+    <sheet name="tech" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="113">
   <si>
     <t>Present, no details</t>
   </si>
@@ -124,9 +136,6 @@
     <t>Global</t>
   </si>
   <si>
-    <t>climate not in EU</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -350,6 +359,24 @@
   </si>
   <si>
     <t>Recalculate EU27 Climate list</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>Ocean</t>
+  </si>
+  <si>
+    <t>Climates</t>
+  </si>
+  <si>
+    <t>Dsb</t>
+  </si>
+  <si>
+    <t>Dsc</t>
   </si>
 </sst>
 </file>
@@ -995,33 +1022,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1029,16 +1056,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -1046,16 +1073,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1063,16 +1090,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1080,16 +1107,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1097,16 +1124,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
         <v>92</v>
-      </c>
-      <c r="D7" t="s">
-        <v>93</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -1114,16 +1141,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -1131,16 +1158,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -1148,16 +1175,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -1165,16 +1192,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -1182,16 +1209,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -1199,16 +1226,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -1216,16 +1243,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -1233,10 +1260,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -1244,16 +1271,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1261,16 +1288,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
         <v>68</v>
       </c>
-      <c r="B17" t="s">
-        <v>69</v>
-      </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -1278,16 +1305,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -1295,16 +1322,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19">
         <v>3</v>
@@ -1312,16 +1339,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -1329,16 +1356,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -1346,16 +1373,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" t="s">
         <v>103</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>104</v>
-      </c>
-      <c r="D22" t="s">
-        <v>105</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1363,16 +1390,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1388,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,17 +1452,17 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="1" t="b">
-        <v>0</v>
+        <v>106</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Climates not in EU" prompt="Select yes to exclude climates that are not in Europe from visualization" xr:uid="{67D655F5-1EE8-45C1-BEA6-D66676F22775}">
           <x14:formula1>
             <xm:f>tech!$J$2:$J$3</xm:f>
@@ -1448,6 +1475,12 @@
           </x14:formula1>
           <xm:sqref>B3</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{482D41D3-29EE-49D4-85AA-B3E82588417B}">
+          <x14:formula1>
+            <xm:f>tech!$J$2:$J$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1455,42 +1488,83 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B4FD27-DD83-404E-B71B-70883D41A962}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
       <c r="J1" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1542,7 +1616,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1593,7 +1667,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>-90</v>
@@ -1639,7 +1713,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>110</v>
@@ -1662,7 +1736,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>-130</v>

</xml_diff>

<commit_message>
Started major modification to code organization. Layers are loaded conditionally. Additional conditions based on configuration file
</commit_message>
<xml_diff>
--- a/Potential.establishment.KG_Configuration.xlsx
+++ b/Potential.establishment.KG_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maioran\Documents\Projects\Potential-establishment-KG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8492B5-D63F-424F-B2FF-1CA8369CD2E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4894C6BF-FCF8-4CF4-B0BE-576EDD74F6BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -18,10 +18,15 @@
     <sheet name="Pest_status_to_be_included" sheetId="2" r:id="rId3"/>
     <sheet name="Host_status_to_be_removed" sheetId="3" r:id="rId4"/>
     <sheet name="Protected_zones" sheetId="7" r:id="rId5"/>
-    <sheet name="Other settings" sheetId="4" r:id="rId6"/>
-    <sheet name="Climates_to_remove" sheetId="8" r:id="rId7"/>
-    <sheet name="tech" sheetId="6" r:id="rId8"/>
+    <sheet name="Protected_zones (2)" sheetId="9" r:id="rId6"/>
+    <sheet name="Other settings" sheetId="4" r:id="rId7"/>
+    <sheet name="Climates_to_remove" sheetId="8" r:id="rId8"/>
+    <sheet name="tech" sheetId="6" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="eu.nuts">tech!$L$2:$L$4</definedName>
+    <definedName name="fao.gaul">tech!$M$2:$M$4</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="116">
   <si>
     <t>Present, no details</t>
   </si>
@@ -172,9 +177,6 @@
     <t>PZ</t>
   </si>
   <si>
-    <t>nuts</t>
-  </si>
-  <si>
     <t>Ireland</t>
   </si>
   <si>
@@ -377,6 +379,18 @@
   </si>
   <si>
     <t>Dsc</t>
+  </si>
+  <si>
+    <t>admin.level</t>
+  </si>
+  <si>
+    <t>eu.nuts</t>
+  </si>
+  <si>
+    <t>Download EPPO host table</t>
+  </si>
+  <si>
+    <t>nuts.level</t>
   </si>
 </sst>
 </file>
@@ -820,7 +834,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,18 +1020,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF26EFA2-9019-4F6D-83AA-2B168DCBB3B9}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1025,30 +1041,88 @@
         <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DF9D14B1-DB73-4BE8-AE1F-455D69047056}">
+          <x14:formula1>
+            <xm:f>tech!$L$2:$L$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1117:E1554</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{02383CB7-DBDA-40A6-AD7E-A61C391434A1}">
+          <x14:formula1>
+            <xm:f>tech!$L$2:$L$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1116</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA593C1E-2A9F-4427-A39B-B6CF4F67A5E1}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1056,16 +1130,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -1073,16 +1147,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1090,16 +1164,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1107,16 +1181,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1124,16 +1198,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
         <v>91</v>
-      </c>
-      <c r="D7" t="s">
-        <v>92</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -1141,16 +1215,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -1158,16 +1232,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -1175,16 +1249,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -1192,16 +1266,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -1209,16 +1283,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -1226,16 +1300,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -1243,16 +1317,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -1260,10 +1334,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -1271,16 +1345,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1288,16 +1362,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
         <v>67</v>
       </c>
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -1305,16 +1379,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -1322,16 +1396,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E19">
         <v>3</v>
@@ -1339,16 +1413,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -1356,16 +1430,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -1373,16 +1447,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" t="s">
         <v>102</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>103</v>
-      </c>
-      <c r="D22" t="s">
-        <v>104</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1390,16 +1464,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1411,12 +1485,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,10 +1526,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1479,7 +1561,7 @@
           <x14:formula1>
             <xm:f>tech!$J$2:$J$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
+          <xm:sqref>B4 B5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1487,39 +1569,42 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B4FD27-DD83-404E-B71B-70883D41A962}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1527,21 +1612,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="M1" sqref="M1:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1564,10 +1650,13 @@
         <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="L1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1592,8 +1681,11 @@
       <c r="J2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1618,8 +1710,11 @@
       <c r="J3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1641,8 +1736,11 @@
       <c r="G4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1665,7 +1763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1688,7 +1786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1711,7 +1809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1734,7 +1832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Reorganization ongoing. protected zone file separated from main configuration file. PZ file in specific pest folder under data/processed folder
</commit_message>
<xml_diff>
--- a/Potential.establishment.KG_Configuration.xlsx
+++ b/Potential.establishment.KG_Configuration.xlsx
@@ -8,20 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maioran\Documents\Projects\Potential-establishment-KG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4894C6BF-FCF8-4CF4-B0BE-576EDD74F6BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0927C0E4-3E13-4DD8-B023-2D92999A6D4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
     <sheet name="Pest_list" sheetId="1" r:id="rId2"/>
     <sheet name="Pest_status_to_be_included" sheetId="2" r:id="rId3"/>
     <sheet name="Host_status_to_be_removed" sheetId="3" r:id="rId4"/>
-    <sheet name="Protected_zones" sheetId="7" r:id="rId5"/>
-    <sheet name="Protected_zones (2)" sheetId="9" r:id="rId6"/>
-    <sheet name="Other settings" sheetId="4" r:id="rId7"/>
-    <sheet name="Climates_to_remove" sheetId="8" r:id="rId8"/>
-    <sheet name="tech" sheetId="6" r:id="rId9"/>
+    <sheet name="Other settings" sheetId="4" r:id="rId5"/>
+    <sheet name="Climates_to_remove" sheetId="8" r:id="rId6"/>
+    <sheet name="tech" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="eu.nuts">tech!$L$2:$L$4</definedName>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Present, no details</t>
   </si>
@@ -174,192 +172,6 @@
     <t>Oceania</t>
   </si>
   <si>
-    <t>PZ</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Ibiza</t>
-  </si>
-  <si>
-    <t>Menorca</t>
-  </si>
-  <si>
-    <t>Cyprus</t>
-  </si>
-  <si>
-    <t>Malta</t>
-  </si>
-  <si>
-    <t>Azores</t>
-  </si>
-  <si>
-    <t>Madeira</t>
-  </si>
-  <si>
-    <t>Kymi</t>
-  </si>
-  <si>
-    <t>Pirkanmaa</t>
-  </si>
-  <si>
-    <t>Häme</t>
-  </si>
-  <si>
-    <t>Satakunta</t>
-  </si>
-  <si>
-    <t>Turku</t>
-  </si>
-  <si>
-    <t>Uusimaa</t>
-  </si>
-  <si>
-    <t>Åland</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Finland</t>
-  </si>
-  <si>
-    <t>Gotland</t>
-  </si>
-  <si>
-    <t>Halland</t>
-  </si>
-  <si>
-    <t>Kalmar</t>
-  </si>
-  <si>
-    <t>Skåne</t>
-  </si>
-  <si>
-    <t>Blekinge</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>PZ_name2</t>
-  </si>
-  <si>
-    <t>Kanta-Häme</t>
-  </si>
-  <si>
-    <t>Päijät-Häme</t>
-  </si>
-  <si>
-    <t>Kymenlaakso</t>
-  </si>
-  <si>
-    <t>Helsinki-Uusimaa</t>
-  </si>
-  <si>
-    <t>NUTS_CODE</t>
-  </si>
-  <si>
-    <t>FI200</t>
-  </si>
-  <si>
-    <t>FI1C2</t>
-  </si>
-  <si>
-    <t>FI1C3</t>
-  </si>
-  <si>
-    <t>FI1C4</t>
-  </si>
-  <si>
-    <t>FI197</t>
-  </si>
-  <si>
-    <t>FI196</t>
-  </si>
-  <si>
-    <t>FI1B1</t>
-  </si>
-  <si>
-    <t>Blekinge County</t>
-  </si>
-  <si>
-    <t>SE221</t>
-  </si>
-  <si>
-    <t>Gotland County</t>
-  </si>
-  <si>
-    <t>Halland County</t>
-  </si>
-  <si>
-    <t>Kalmar County</t>
-  </si>
-  <si>
-    <t>Skåne County</t>
-  </si>
-  <si>
-    <t>ES533</t>
-  </si>
-  <si>
-    <t>Eivissa i Formentera</t>
-  </si>
-  <si>
-    <t>ES531</t>
-  </si>
-  <si>
-    <t>PT200</t>
-  </si>
-  <si>
-    <t>Região Autónoma dos Açores</t>
-  </si>
-  <si>
-    <t>Região Autónoma da Madeira</t>
-  </si>
-  <si>
-    <t>PT300</t>
-  </si>
-  <si>
-    <t>SE214</t>
-  </si>
-  <si>
-    <t>SE231</t>
-  </si>
-  <si>
-    <t>SE213</t>
-  </si>
-  <si>
-    <t>SE224</t>
-  </si>
-  <si>
-    <t>IE</t>
-  </si>
-  <si>
-    <t>CY</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>UKN0</t>
-  </si>
-  <si>
-    <t>Northern Ireland</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
     <t>Recalculate EU27 Climate list</t>
   </si>
   <si>
@@ -381,16 +193,13 @@
     <t>Dsc</t>
   </si>
   <si>
-    <t>admin.level</t>
-  </si>
-  <si>
     <t>eu.nuts</t>
   </si>
   <si>
     <t>Download EPPO host table</t>
   </si>
   <si>
-    <t>nuts.level</t>
+    <t>Include protected zones</t>
   </si>
 </sst>
 </file>
@@ -1019,478 +828,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF26EFA2-9019-4F6D-83AA-2B168DCBB3B9}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DF9D14B1-DB73-4BE8-AE1F-455D69047056}">
-          <x14:formula1>
-            <xm:f>tech!$L$2:$L$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>E1117:E1554</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{02383CB7-DBDA-40A6-AD7E-A61C391434A1}">
-          <x14:formula1>
-            <xm:f>tech!$L$2:$L$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E1116</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA593C1E-2A9F-4427-A39B-B6CF4F67A5E1}">
-  <dimension ref="A1:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" t="s">
-        <v>102</v>
-      </c>
-      <c r="D22" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>101</v>
-      </c>
-      <c r="B23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" t="s">
-        <v>101</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,7 +868,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
@@ -1534,9 +876,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1561,7 +911,7 @@
           <x14:formula1>
             <xm:f>tech!$J$2:$J$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B4 B5</xm:sqref>
+          <xm:sqref>B4:B6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1569,12 +919,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B4FD27-DD83-404E-B71B-70883D41A962}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,27 +934,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1612,7 +962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
@@ -1650,10 +1000,10 @@
         <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="L1" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reorganization of code. Working on including different administrative layers.
</commit_message>
<xml_diff>
--- a/Potential.establishment.KG_Configuration.xlsx
+++ b/Potential.establishment.KG_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maioran\Documents\Projects\Potential-establishment-KG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0927C0E4-3E13-4DD8-B023-2D92999A6D4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72597F86-8FF5-4EE7-A397-2B1496E162C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="3570" windowWidth="13995" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>Status to be removed</t>
   </si>
   <si>
-    <t>Leptinotarsa decemlineata</t>
-  </si>
-  <si>
     <t>Status to be included</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>Include protected zones</t>
+  </si>
+  <si>
+    <t>Dendrolimus spectabilis</t>
   </si>
 </sst>
 </file>
@@ -682,10 +682,10 @@
     </row>
     <row r="5" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -735,7 +735,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -761,7 +761,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -860,34 +860,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -923,7 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B4FD27-DD83-404E-B71B-70883D41A962}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
@@ -934,27 +934,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -979,36 +979,36 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>-180</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>-180</v>
@@ -1058,7 +1058,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>30</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>80</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>-90</v>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>-35</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>110</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9">
         <v>-130</v>

</xml_diff>

<commit_message>
Version ready for testing
</commit_message>
<xml_diff>
--- a/Potential.establishment.KG_Configuration.xlsx
+++ b/Potential.establishment.KG_Configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maioran\Documents\Projects\Potential-establishment-KG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72597F86-8FF5-4EE7-A397-2B1496E162C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F208858-5639-4323-8D4C-2A5F348ECB79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3570" windowWidth="13995" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -717,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -793,7 +793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -832,7 +832,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +863,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
EFSA Climate Suitability Tool 0.9: Included protected zones. Tool ready for testing.
</commit_message>
<xml_diff>
--- a/Potential.establishment.KG_Configuration.xlsx
+++ b/Potential.establishment.KG_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maioran\Documents\Projects\Potential-establishment-KG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F208858-5639-4323-8D4C-2A5F348ECB79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DE508A-3D3D-4C5C-94FB-A6C787AA6BA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -793,7 +793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +887,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on administrative layers and tables
</commit_message>
<xml_diff>
--- a/Potential.establishment.KG_Configuration.xlsx
+++ b/Potential.establishment.KG_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maioran\Documents\Projects\Potential-establishment-KG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DE508A-3D3D-4C5C-94FB-A6C787AA6BA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE25539-D8DD-449D-8B50-9FE8A1F9372F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -199,7 +199,7 @@
     <t>Include protected zones</t>
   </si>
   <si>
-    <t>Dendrolimus spectabilis</t>
+    <t>Conotrachelus nenuphar</t>
   </si>
 </sst>
 </file>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +855,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -887,7 +887,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -966,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,13 +1190,13 @@
         <v>-130</v>
       </c>
       <c r="C9">
-        <v>-60</v>
+        <v>-50</v>
       </c>
       <c r="D9">
         <v>20</v>
       </c>
       <c r="E9">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F9">
         <v>5</v>

</xml_diff>

<commit_message>
Start working on Markdown report
</commit_message>
<xml_diff>
--- a/Potential.establishment.KG_Configuration.xlsx
+++ b/Potential.establishment.KG_Configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maioran\Documents\Projects\Potential-establishment-KG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE25539-D8DD-449D-8B50-9FE8A1F9372F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EC5169-ECB5-4AC2-9239-4811D89FE46F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -175,9 +175,6 @@
     <t>Boolean</t>
   </si>
   <si>
-    <t>ET</t>
-  </si>
-  <si>
     <t>Ocean</t>
   </si>
   <si>
@@ -199,7 +196,10 @@
     <t>Include protected zones</t>
   </si>
   <si>
-    <t>Conotrachelus nenuphar</t>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Elasmopalpus lignosellus</t>
   </si>
 </sst>
 </file>
@@ -646,14 +646,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="109.28515625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.33203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -661,10 +661,10 @@
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -672,7 +672,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -680,7 +680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -688,7 +688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -696,7 +696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -717,23 +717,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="42.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
@@ -752,34 +752,34 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="28.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -795,29 +795,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -832,17 +832,17 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -850,23 +850,23 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -874,17 +874,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>31</v>
@@ -903,7 +903,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry!" error="Please select a Region from the list" promptTitle="Regions" prompt="Please select a Region from the list" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
-            <xm:f>tech!$A$2:$A$9</xm:f>
+            <xm:f>tech!$A$2:$A$50</xm:f>
           </x14:formula1>
           <xm:sqref>B3</xm:sqref>
         </x14:dataValidation>
@@ -921,40 +921,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B4FD27-DD83-404E-B71B-70883D41A962}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -964,20 +959,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1003,10 +998,10 @@
         <v>43</v>
       </c>
       <c r="L1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1035,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1064,7 +1059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1090,7 +1085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1113,7 +1108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1136,18 +1131,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="B7">
-        <v>-35</v>
+        <v>-30</v>
       </c>
       <c r="C7">
         <v>50</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>75</v>
@@ -1159,7 +1154,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1182,7 +1177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1202,6 +1197,29 @@
         <v>5</v>
       </c>
       <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>-85</v>
+      </c>
+      <c r="C10">
+        <v>-65</v>
+      </c>
+      <c r="D10">
+        <v>-20</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
         <v>5</v>
       </c>
     </row>

</xml_diff>